<commit_message>
data parsing for dell xml inventory and xlsx export implementation
</commit_message>
<xml_diff>
--- a/dell/HardwareInventory.xml_report.xlsx
+++ b/dell/HardwareInventory.xml_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
   <si>
     <t>ServiceTag</t>
   </si>
@@ -22,13 +22,127 @@
     <t>8YN4J82</t>
   </si>
   <si>
-    <t>CPUs model</t>
+    <t>CPU model</t>
   </si>
   <si>
     <t>Intel(R) Xeon(R) CPU E5-2620 v3 @ 2.40GHz</t>
   </si>
   <si>
-    <t>HDD serials</t>
+    <t>PCI device</t>
+  </si>
+  <si>
+    <t>C610/X99 series chipset sSATA Controller [AHCI mode]</t>
+  </si>
+  <si>
+    <t>C610/X99 series chipset 6-Port SATA Controller [AHCI mode]</t>
+  </si>
+  <si>
+    <t>ISP2532-based 8Gb Fibre Channel to PCI Express HBA</t>
+  </si>
+  <si>
+    <t>Terminator 2x/i</t>
+  </si>
+  <si>
+    <t>C610/X99 series chipset LPC Controller</t>
+  </si>
+  <si>
+    <t>Ethernet 10G 4P X520/I350 rNDC</t>
+  </si>
+  <si>
+    <t>I350 Gigabit Network Connection</t>
+  </si>
+  <si>
+    <t>Renesas Technology Corp.</t>
+  </si>
+  <si>
+    <t>C610/X99 series chipset PCI Express Root Port #1</t>
+  </si>
+  <si>
+    <t>C610/X99 series chipset PCI Express Root Port #8</t>
+  </si>
+  <si>
+    <t>C610/X99 series chipset PCI Express Root Port #5</t>
+  </si>
+  <si>
+    <t>PERC H330 Mini</t>
+  </si>
+  <si>
+    <t>C610/X99 series chipset USB Enhanced Host Controller #1</t>
+  </si>
+  <si>
+    <t>C610/X99 series chipset USB Enhanced Host Controller #2</t>
+  </si>
+  <si>
+    <t>G200eR2</t>
+  </si>
+  <si>
+    <t>System memory size</t>
+  </si>
+  <si>
+    <t>65536</t>
+  </si>
+  <si>
+    <t>Memory serial</t>
+  </si>
+  <si>
+    <t>413C1F90</t>
+  </si>
+  <si>
+    <t>413C1F7E</t>
+  </si>
+  <si>
+    <t>413C1F7C</t>
+  </si>
+  <si>
+    <t>413C1F7F</t>
+  </si>
+  <si>
+    <t>413C1F96</t>
+  </si>
+  <si>
+    <t>413C1F5C</t>
+  </si>
+  <si>
+    <t>413C1F49</t>
+  </si>
+  <si>
+    <t>413C0CCA</t>
+  </si>
+  <si>
+    <t>Memory module part number</t>
+  </si>
+  <si>
+    <t>M393A1G43DB0-CPB</t>
+  </si>
+  <si>
+    <t>Memory slot</t>
+  </si>
+  <si>
+    <t>DIMM.Socket.A1</t>
+  </si>
+  <si>
+    <t>DIMM.Socket.A2</t>
+  </si>
+  <si>
+    <t>DIMM.Socket.A3</t>
+  </si>
+  <si>
+    <t>DIMM.Socket.A4</t>
+  </si>
+  <si>
+    <t>DIMM.Socket.B1</t>
+  </si>
+  <si>
+    <t>DIMM.Socket.B2</t>
+  </si>
+  <si>
+    <t>DIMM.Socket.B3</t>
+  </si>
+  <si>
+    <t>DIMM.Socket.B4</t>
+  </si>
+  <si>
+    <t>HDD serial</t>
   </si>
   <si>
     <t>S4204BFG</t>
@@ -37,13 +151,19 @@
     <t>S4204B53</t>
   </si>
   <si>
+    <t>HDD model</t>
+  </si>
+  <si>
+    <t>ST300MM0008</t>
+  </si>
+  <si>
     <t>HDD fw</t>
   </si>
   <si>
     <t>TT31</t>
   </si>
   <si>
-    <t>HDD slots</t>
+    <t>HDD slot population</t>
   </si>
   <si>
     <t>0</t>
@@ -52,16 +172,31 @@
     <t>1</t>
   </si>
   <si>
-    <t>System memory size</t>
-  </si>
-  <si>
-    <t>65536</t>
-  </si>
-  <si>
-    <t>System memory modules</t>
-  </si>
-  <si>
-    <t>M393A1G43DB0-CPB</t>
+    <t>PSU part number</t>
+  </si>
+  <si>
+    <t>0V1YJ6A00</t>
+  </si>
+  <si>
+    <t>PSU serial</t>
+  </si>
+  <si>
+    <t>CN1797257U45SL</t>
+  </si>
+  <si>
+    <t>CN1797257U45TG</t>
+  </si>
+  <si>
+    <t>PSU model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWR SPLY,750W,RDNT,DELTA      </t>
+  </si>
+  <si>
+    <t>PSU fw</t>
+  </si>
+  <si>
+    <t>00.24.71</t>
   </si>
 </sst>
 </file>
@@ -393,99 +528,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+    <col min="3" max="3" width="58.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="30.7109375" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="C13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
+    <row r="14" spans="1:15">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="15" spans="1:15">
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
-        <v>15</v>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>